<commit_message>
Envio de img pelo whats
</commit_message>
<xml_diff>
--- a/contatos.xlsx
+++ b/contatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HomePC\Desktop\ProjetoMensageria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4432B25-7EC0-41DC-976E-1EF2C7672479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE160C9B-6F99-41F3-8C63-50FC0D451A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="4215" windowWidth="28800" windowHeight="11385" xr2:uid="{162268BA-26AC-4B4F-817B-1B5020E7D980}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{162268BA-26AC-4B4F-817B-1B5020E7D980}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Vinicius</t>
-  </si>
-  <si>
-    <t>Manuela</t>
-  </si>
-  <si>
-    <t>Kaiky</t>
   </si>
   <si>
     <t>Pessoa</t>
@@ -54,12 +48,6 @@
   </si>
   <si>
     <t>5518996932702</t>
-  </si>
-  <si>
-    <t>5518997031009</t>
-  </si>
-  <si>
-    <t>5518997168462</t>
   </si>
 </sst>
 </file>
@@ -412,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F02907F-5365-4B15-9E2D-73F48973C01D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,10 +413,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,23 +424,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>